<commit_message>
fix: multi threading and style of table
</commit_message>
<xml_diff>
--- a/static/downloads/covid 19 treatment theory.xlsx
+++ b/static/downloads/covid 19 treatment theory.xlsx
@@ -451,7 +451,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Saleh A Alqahtani, Jörn M Schattenberg, Saleh A Alqahtani, Saleh A Alqahtani, Jörn M Schattenberg</t>
+          <t>Saleh A Alqahtani, 
+Jörn M Schattenberg, 
+Saleh A Alqahtani, 
+Saleh A Alqahtani, 
+Jörn M Schattenberg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -529,7 +533,35 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Zhi-Yong Li, Tuya, Hai-Tao Li, Jiang He, Quesheng, Guang-Ping Dong, Ming-Shuo Zhang, Jian-Qin Liu, Xiu-Lan Huang, Xiao-Rong Wang, Makabel Bolat, Xin Feng, Fang-Bo Zhang, Feng Jiang, Zhi-Yong Li, Zhi-Yong Li, Tuya, Hai-Tao Li, Jiang He, Quesheng, Guang-Ping Dong, Ming-Shuo Zhang, Jian-Qin Liu, Xiu-Lan Huang, Xiao-Rong Wang, Makabel Bolat, Xin Feng, Fang-Bo Zhang, Feng Jiang</t>
+          <t>Zhi-Yong Li, 
+Tuya, 
+Hai-Tao Li, 
+Jiang He, 
+Quesheng, 
+Guang-Ping Dong, 
+Ming-Shuo Zhang, 
+Jian-Qin Liu, 
+Xiu-Lan Huang, 
+Xiao-Rong Wang, 
+Makabel Bolat, 
+Xin Feng, 
+Fang-Bo Zhang, 
+Feng Jiang, 
+Zhi-Yong Li, 
+Zhi-Yong Li, 
+Tuya, 
+Hai-Tao Li, 
+Jiang He, 
+Quesheng, 
+Guang-Ping Dong, 
+Ming-Shuo Zhang, 
+Jian-Qin Liu, 
+Xiu-Lan Huang, 
+Xiao-Rong Wang, 
+Makabel Bolat, 
+Xin Feng, 
+Fang-Bo Zhang, 
+Feng Jiang</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -589,7 +621,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>James R Vallerand, Ryan E Rhodes, Gordan J Walker, Kerry S Courneya, James R Vallerand, James R Vallerand, Ryan E Rhodes, Gordan J Walker, Kerry S Courneya</t>
+          <t>James R Vallerand, 
+Ryan E Rhodes, 
+Gordan J Walker, 
+Kerry S Courneya, 
+James R Vallerand, 
+James R Vallerand, 
+Ryan E Rhodes, 
+Gordan J Walker, 
+Kerry S Courneya</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>

</xml_diff>

<commit_message>
fix: issue in author names
</commit_message>
<xml_diff>
--- a/static/downloads/covid 19 treatment theory.xlsx
+++ b/static/downloads/covid 19 treatment theory.xlsx
@@ -452,9 +452,6 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>Saleh A Alqahtani, 
-Jörn M Schattenberg, 
-Saleh A Alqahtani, 
-Saleh A Alqahtani, 
 Jörn M Schattenberg</t>
         </is>
       </c>
@@ -546,21 +543,6 @@
 Makabel Bolat, 
 Xin Feng, 
 Fang-Bo Zhang, 
-Feng Jiang, 
-Zhi-Yong Li, 
-Zhi-Yong Li, 
-Tuya, 
-Hai-Tao Li, 
-Jiang He, 
-Quesheng, 
-Guang-Ping Dong, 
-Ming-Shuo Zhang, 
-Jian-Qin Liu, 
-Xiu-Lan Huang, 
-Xiao-Rong Wang, 
-Makabel Bolat, 
-Xin Feng, 
-Fang-Bo Zhang, 
 Feng Jiang</t>
         </is>
       </c>
@@ -622,11 +604,6 @@
       <c r="E4" t="inlineStr">
         <is>
           <t>James R Vallerand, 
-Ryan E Rhodes, 
-Gordan J Walker, 
-Kerry S Courneya, 
-James R Vallerand, 
-James R Vallerand, 
 Ryan E Rhodes, 
 Gordan J Walker, 
 Kerry S Courneya</t>

</xml_diff>